<commit_message>
Refactoring and changes to buy/sell limits
Extracted some code to methods and updated buy/sell limits. Updated test
code to match n ew buy/sell limits.
</commit_message>
<xml_diff>
--- a/test/test_data.xlsx
+++ b/test/test_data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12468" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12468"/>
   </bookViews>
   <sheets>
     <sheet name="Test Data" sheetId="3" r:id="rId1"/>
@@ -263,7 +263,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -273,6 +273,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="13">
     <cellStyle name="1_Supplied Input (Vendor/Customer/Etc.)" xfId="1"/>
@@ -531,8 +532,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O59"/>
   <sheetViews>
-    <sheetView topLeftCell="B35" workbookViewId="0">
-      <selection activeCell="I46" sqref="I46"/>
+    <sheetView tabSelected="1" topLeftCell="B41" workbookViewId="0">
+      <selection activeCell="H59" sqref="H59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -597,7 +598,7 @@
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="6"/>
+      <c r="A2" s="9"/>
       <c r="B2" s="6">
         <v>13000</v>
       </c>
@@ -635,8 +636,8 @@
         <v>23</v>
       </c>
       <c r="F3" s="6">
-        <f>$D3 * 0.1</f>
-        <v>100</v>
+        <f>$D3 * 0.2</f>
+        <v>200</v>
       </c>
       <c r="G3" s="6">
         <f>$B3 - 2</f>
@@ -647,8 +648,8 @@
         <v>11700</v>
       </c>
       <c r="I3" s="6">
-        <f>ROUNDDOWN($F3/$H3, 5)</f>
-        <v>8.5400000000000007E-3</v>
+        <f t="shared" ref="I3:I9" si="0">ROUNDDOWN($F3/$H3, 5)</f>
+        <v>1.7090000000000001E-2</v>
       </c>
       <c r="J3" s="6" t="s">
         <v>7</v>
@@ -669,47 +670,47 @@
         <v>11703</v>
       </c>
       <c r="D4" s="6">
-        <f>$D3 - $F3</f>
-        <v>900</v>
+        <f t="shared" ref="D4:D9" si="1">$D3 - $F3</f>
+        <v>800</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>24</v>
       </c>
       <c r="F4" s="6">
-        <f>$D4 * 0.1</f>
-        <v>90</v>
+        <f>$D4 * 0.2</f>
+        <v>160</v>
       </c>
       <c r="G4" s="6">
-        <f>$H3 - ($H3 * 0.01)</f>
-        <v>11583</v>
+        <f>$H3 - ($H3 * 0.005)</f>
+        <v>11641.5</v>
       </c>
       <c r="H4" s="6">
-        <f>ROUND(MIN($G4, $B4), 0) - 2</f>
-        <v>11581</v>
+        <f t="shared" ref="H4:H9" si="2">ROUND(MIN($G4, $B4), 0) - 2</f>
+        <v>11640</v>
       </c>
       <c r="I4" s="6">
-        <f>ROUNDDOWN($F4/$H4, 5)</f>
-        <v>7.77E-3</v>
+        <f t="shared" si="0"/>
+        <v>1.374E-2</v>
       </c>
       <c r="J4" s="6">
         <f>$H3 + ($H3* 0.005)</f>
         <v>11758.5</v>
       </c>
       <c r="K4">
-        <f>ROUND(MAX($J4,$C4), 0) + 2</f>
+        <f t="shared" ref="K4:K9" si="3">ROUND(MAX($J4,$C4), 0) + 2</f>
         <v>11761</v>
       </c>
       <c r="L4">
-        <f>$I3</f>
-        <v>8.5400000000000007E-3</v>
+        <f t="shared" ref="L4:L9" si="4">$I3</f>
+        <v>1.7090000000000001E-2</v>
       </c>
       <c r="N4" s="5">
-        <f>L4 * ($K4 - $H3)</f>
-        <v>0.52094000000000007</v>
+        <f t="shared" ref="N4:N9" si="5">L4 * ($K4 - $H3)</f>
+        <v>1.0424900000000001</v>
       </c>
       <c r="O4" s="7">
-        <f>$N4 / $F3</f>
-        <v>5.2094000000000003E-3</v>
+        <f t="shared" ref="O4:O9" si="6">$N4 / $F3</f>
+        <v>5.2124500000000004E-3</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
@@ -721,252 +722,252 @@
         <v>11583</v>
       </c>
       <c r="D5" s="6">
-        <f>$D4 - $F4</f>
-        <v>810</v>
+        <f t="shared" si="1"/>
+        <v>640</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>24</v>
       </c>
       <c r="F5" s="6">
-        <f>$D5 * 0.1</f>
-        <v>81</v>
+        <f>$D5 * 0.2</f>
+        <v>128</v>
       </c>
       <c r="G5" s="6">
-        <f>$H4 - ($H4 * 0.02)</f>
-        <v>11349.38</v>
+        <f>$H4 - ($H4 * 0.01)</f>
+        <v>11523.6</v>
       </c>
       <c r="H5" s="6">
-        <f>ROUND(MIN($G5, $B5), 0) - 2</f>
-        <v>11347</v>
+        <f t="shared" si="2"/>
+        <v>11522</v>
       </c>
       <c r="I5" s="6">
-        <f>ROUNDDOWN($F5/$H5, 5)</f>
-        <v>7.1300000000000001E-3</v>
+        <f t="shared" si="0"/>
+        <v>1.11E-2</v>
       </c>
       <c r="J5" s="6">
         <f>$H4 + ($H4* 0.005)</f>
-        <v>11638.905000000001</v>
+        <v>11698.2</v>
       </c>
       <c r="K5">
-        <f>ROUND(MAX($J5,$C5), 0) + 2</f>
-        <v>11641</v>
+        <f t="shared" si="3"/>
+        <v>11700</v>
       </c>
       <c r="L5">
-        <f>$I4</f>
-        <v>7.77E-3</v>
+        <f t="shared" si="4"/>
+        <v>1.374E-2</v>
       </c>
       <c r="N5" s="5">
-        <f>L5 * ($K5 - $H4)</f>
-        <v>0.4662</v>
+        <f t="shared" si="5"/>
+        <v>0.82440000000000002</v>
       </c>
       <c r="O5" s="7">
-        <f>$N5 / $F4</f>
-        <v>5.1799999999999997E-3</v>
+        <f t="shared" si="6"/>
+        <v>5.1525E-3</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="6"/>
       <c r="B6" s="6">
-        <v>11348</v>
+        <v>11465</v>
       </c>
       <c r="C6" s="6">
-        <v>11349</v>
+        <v>11466</v>
       </c>
       <c r="D6" s="6">
-        <f>$D5 - $F5</f>
-        <v>729</v>
+        <f t="shared" si="1"/>
+        <v>512</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>24</v>
       </c>
       <c r="F6" s="6">
-        <f>$D6 * 0.1</f>
-        <v>72.900000000000006</v>
+        <f>$D6 * 0.2</f>
+        <v>102.4</v>
       </c>
       <c r="G6" s="6">
-        <f>$H5 - ($H5 * 0.005)</f>
-        <v>11290.264999999999</v>
+        <f>$H5 - ($H5 * 0.015)</f>
+        <v>11349.17</v>
       </c>
       <c r="H6" s="6">
-        <f>ROUND(MIN($G6, $B6), 0) - 2</f>
-        <v>11288</v>
+        <f t="shared" si="2"/>
+        <v>11347</v>
       </c>
       <c r="I6" s="6">
-        <f>ROUNDDOWN($F6/$H6, 5)</f>
-        <v>6.45E-3</v>
+        <f t="shared" si="0"/>
+        <v>9.0200000000000002E-3</v>
       </c>
       <c r="J6" s="6">
-        <f>$H5 + ($H5* 0.01)</f>
-        <v>11460.47</v>
+        <f>$H5 + ($H5* 0.005)</f>
+        <v>11579.61</v>
       </c>
       <c r="K6">
-        <f>ROUND(MAX($J6,$C6), 0) + 2</f>
-        <v>11462</v>
+        <f t="shared" si="3"/>
+        <v>11582</v>
       </c>
       <c r="L6">
-        <f>$I5</f>
-        <v>7.1300000000000001E-3</v>
+        <f t="shared" si="4"/>
+        <v>1.11E-2</v>
       </c>
       <c r="N6" s="5">
-        <f>L6 * ($K6 - $H5)</f>
-        <v>0.81994999999999996</v>
+        <f t="shared" si="5"/>
+        <v>0.66600000000000004</v>
       </c>
       <c r="O6" s="7">
-        <f>$N6 / $F5</f>
-        <v>1.012283950617284E-2</v>
+        <f t="shared" si="6"/>
+        <v>5.2031250000000003E-3</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B7" s="6">
-        <v>11289</v>
+        <v>11291</v>
       </c>
       <c r="C7" s="6">
-        <v>11290</v>
+        <v>11292</v>
       </c>
       <c r="D7" s="6">
-        <f>$D6 - $F6</f>
-        <v>656.1</v>
+        <f t="shared" si="1"/>
+        <v>409.6</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>24</v>
       </c>
       <c r="F7" s="6">
-        <f>$D7 * 0.1</f>
-        <v>65.61</v>
+        <f>$D7 * 0.15</f>
+        <v>61.44</v>
       </c>
       <c r="G7" s="6">
-        <f>$H6 - ($H6 * 0.01)</f>
-        <v>11175.12</v>
+        <f>$H6 - ($H6 * 0.005)</f>
+        <v>11290.264999999999</v>
       </c>
       <c r="H7" s="6">
-        <f>ROUND(MIN($G7, $B7), 0) - 2</f>
-        <v>11173</v>
+        <f t="shared" si="2"/>
+        <v>11288</v>
       </c>
       <c r="I7" s="6">
-        <f>ROUNDDOWN($F7/$H7, 5)</f>
-        <v>5.8700000000000002E-3</v>
+        <f t="shared" si="0"/>
+        <v>5.4400000000000004E-3</v>
       </c>
       <c r="J7" s="6">
-        <f>$H6 + ($H6* 0.005)</f>
-        <v>11344.44</v>
+        <f>$H6 + ($H6* 0.01)</f>
+        <v>11460.47</v>
       </c>
       <c r="K7">
-        <f>ROUND(MAX($J7,$C7), 0) + 2</f>
-        <v>11346</v>
+        <f t="shared" si="3"/>
+        <v>11462</v>
       </c>
       <c r="L7">
-        <f>$I6</f>
-        <v>6.45E-3</v>
+        <f t="shared" si="4"/>
+        <v>9.0200000000000002E-3</v>
       </c>
       <c r="N7" s="5">
-        <f>L7 * ($K7 - $H6)</f>
-        <v>0.37409999999999999</v>
+        <f t="shared" si="5"/>
+        <v>1.0373000000000001</v>
       </c>
       <c r="O7" s="7">
-        <f>$N7 / $F6</f>
-        <v>5.1316872427983537E-3</v>
+        <f t="shared" si="6"/>
+        <v>1.0129882812500001E-2</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B8" s="6">
-        <v>11174</v>
+        <v>11232</v>
       </c>
       <c r="C8" s="6">
-        <v>11175</v>
+        <v>11233</v>
       </c>
       <c r="D8" s="6">
-        <f>$D7 - $F7</f>
-        <v>590.49</v>
+        <f t="shared" si="1"/>
+        <v>348.16</v>
       </c>
       <c r="E8" s="6" t="s">
         <v>24</v>
       </c>
       <c r="F8" s="6">
-        <f>$D8 * 0.1</f>
-        <v>59.049000000000007</v>
+        <f>$D8 * 0.15</f>
+        <v>52.224000000000004</v>
       </c>
       <c r="G8" s="6">
-        <f>$H7 - ($H7 * 0.02)</f>
-        <v>10949.54</v>
+        <f>$H7 - ($H7 * 0.005)</f>
+        <v>11231.56</v>
       </c>
       <c r="H8" s="6">
-        <f>ROUND(MIN($G8, $B8), 0) - 2</f>
-        <v>10948</v>
+        <f t="shared" si="2"/>
+        <v>11230</v>
       </c>
       <c r="I8" s="6">
-        <f>ROUNDDOWN($F8/$H8, 5)</f>
-        <v>5.3899999999999998E-3</v>
+        <f t="shared" si="0"/>
+        <v>4.6499999999999996E-3</v>
       </c>
       <c r="J8" s="6">
         <f>$H7 + ($H7* 0.005)</f>
-        <v>11228.865</v>
+        <v>11344.44</v>
       </c>
       <c r="K8">
-        <f>ROUND(MAX($J8,$C8), 0) + 2</f>
-        <v>11231</v>
+        <f t="shared" si="3"/>
+        <v>11346</v>
       </c>
       <c r="L8">
-        <f>$I7</f>
-        <v>5.8700000000000002E-3</v>
+        <f t="shared" si="4"/>
+        <v>5.4400000000000004E-3</v>
       </c>
       <c r="N8" s="5">
-        <f>L8 * ($K8 - $H7)</f>
-        <v>0.34045999999999998</v>
+        <f t="shared" si="5"/>
+        <v>0.31552000000000002</v>
       </c>
       <c r="O8" s="7">
-        <f>$N8 / $F7</f>
-        <v>5.1891479957323575E-3</v>
+        <f t="shared" si="6"/>
+        <v>5.1354166666666675E-3</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B9" s="6">
-        <v>10949</v>
+        <v>11174</v>
       </c>
       <c r="C9" s="6">
-        <v>10950</v>
+        <v>11175</v>
       </c>
       <c r="D9" s="6">
-        <f>$D8 - $F8</f>
-        <v>531.44100000000003</v>
+        <f t="shared" si="1"/>
+        <v>295.93600000000004</v>
       </c>
       <c r="E9" s="6" t="s">
         <v>24</v>
       </c>
       <c r="F9" s="6">
-        <f>$D9 * 0.1</f>
-        <v>53.144100000000009</v>
+        <f>$D9 * 0.15</f>
+        <v>44.390400000000007</v>
       </c>
       <c r="G9" s="6">
-        <f>$H8 - ($H8 * 0.005)</f>
-        <v>10893.26</v>
+        <f>$H8 - ($H8 * 0.01)</f>
+        <v>11117.7</v>
       </c>
       <c r="H9" s="6">
-        <f>ROUND(MIN($G9, $B9), 0) - 2</f>
-        <v>10891</v>
+        <f t="shared" si="2"/>
+        <v>11116</v>
       </c>
       <c r="I9" s="6">
-        <f>ROUNDDOWN($F9/$H9, 5)</f>
-        <v>4.8700000000000002E-3</v>
+        <f t="shared" si="0"/>
+        <v>3.9899999999999996E-3</v>
       </c>
       <c r="J9" s="6">
-        <f>$H8 + ($H8* 0.01)</f>
-        <v>11057.48</v>
+        <f>$H8 + ($H8* 0.005)</f>
+        <v>11286.15</v>
       </c>
       <c r="K9">
-        <f>ROUND(MAX($J9,$C9), 0) + 2</f>
-        <v>11059</v>
+        <f t="shared" si="3"/>
+        <v>11288</v>
       </c>
       <c r="L9">
-        <f>$I8</f>
-        <v>5.3899999999999998E-3</v>
+        <f t="shared" si="4"/>
+        <v>4.6499999999999996E-3</v>
       </c>
       <c r="N9" s="5">
-        <f>L9 * ($K9 - $H8)</f>
-        <v>0.59828999999999999</v>
+        <f t="shared" si="5"/>
+        <v>0.2697</v>
       </c>
       <c r="O9" s="7">
-        <f>$N9 / $F8</f>
-        <v>1.0132093684905755E-2</v>
+        <f t="shared" si="6"/>
+        <v>5.1642922794117646E-3</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
@@ -1052,8 +1053,8 @@
         <v>23</v>
       </c>
       <c r="F18" s="6">
-        <f>$D18 * 0.1</f>
-        <v>100</v>
+        <f>$D18 * 0.2</f>
+        <v>200</v>
       </c>
       <c r="G18" s="6">
         <f>$B18 - 2</f>
@@ -1064,8 +1065,8 @@
         <v>11700</v>
       </c>
       <c r="I18" s="6">
-        <f>ROUNDDOWN($F18/$H18, 5)</f>
-        <v>8.5400000000000007E-3</v>
+        <f t="shared" ref="I18:I24" si="7">ROUNDDOWN($F18/$H18, 5)</f>
+        <v>1.7090000000000001E-2</v>
       </c>
       <c r="J18" s="6" t="s">
         <v>7</v>
@@ -1080,310 +1081,310 @@
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="6"/>
       <c r="B19" s="6">
-        <v>11550</v>
+        <v>11000</v>
       </c>
       <c r="C19" s="6">
-        <v>11780</v>
+        <v>11001</v>
       </c>
       <c r="D19" s="6">
-        <f>$D18 - $F18</f>
-        <v>900</v>
+        <f t="shared" ref="D19:D24" si="8">$D18 - $F18</f>
+        <v>800</v>
       </c>
       <c r="E19" s="6" t="s">
         <v>24</v>
       </c>
       <c r="F19" s="6">
-        <f>$D19 * 0.1</f>
-        <v>90</v>
+        <f>$D19 * 0.2</f>
+        <v>160</v>
       </c>
       <c r="G19" s="6">
-        <f>$H18 - ($H18 * 0.01)</f>
-        <v>11583</v>
+        <f>$H18 - ($H18 * 0.005)</f>
+        <v>11641.5</v>
       </c>
       <c r="H19" s="6">
-        <f>ROUND(MIN($G19, $B19), 0) - 2</f>
-        <v>11548</v>
+        <f t="shared" ref="H19:H24" si="9">ROUND(MIN($G19, $B19), 0) - 2</f>
+        <v>10998</v>
       </c>
       <c r="I19" s="6">
-        <f>ROUNDDOWN($F19/$H19, 5)</f>
-        <v>7.79E-3</v>
+        <f t="shared" si="7"/>
+        <v>1.4540000000000001E-2</v>
       </c>
       <c r="J19" s="6">
         <f>$H18 + ($H18* 0.005)</f>
         <v>11758.5</v>
       </c>
       <c r="K19">
-        <f>ROUND(MAX($J19,$C19), 0) + 2</f>
-        <v>11782</v>
+        <f t="shared" ref="K19:K24" si="10">ROUND(MAX($J19,$C19), 0) + 2</f>
+        <v>11761</v>
       </c>
       <c r="L19">
-        <f>$I18</f>
-        <v>8.5400000000000007E-3</v>
+        <f t="shared" ref="L19:L24" si="11">$I18</f>
+        <v>1.7090000000000001E-2</v>
       </c>
       <c r="N19" s="5">
-        <f>L19 * ($K19 - $H18)</f>
-        <v>0.70028000000000001</v>
+        <f t="shared" ref="N19:N24" si="12">L19 * ($K19 - $H18)</f>
+        <v>1.0424900000000001</v>
       </c>
       <c r="O19" s="7">
-        <f>$N19 / $F18</f>
-        <v>7.0028E-3</v>
+        <f t="shared" ref="O19:O24" si="13">$N19 / $F18</f>
+        <v>5.2124500000000004E-3</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="6"/>
       <c r="B20" s="6">
-        <v>11300</v>
+        <v>10850</v>
       </c>
       <c r="C20" s="6">
-        <v>11650</v>
+        <v>10851</v>
       </c>
       <c r="D20" s="6">
-        <f>$D19 - $F19</f>
-        <v>810</v>
+        <f t="shared" si="8"/>
+        <v>640</v>
       </c>
       <c r="E20" s="6" t="s">
         <v>24</v>
       </c>
       <c r="F20" s="6">
-        <f>$D20 * 0.1</f>
-        <v>81</v>
+        <f>$D20 * 0.2</f>
+        <v>128</v>
       </c>
       <c r="G20" s="6">
-        <f>$H19 - ($H19 * 0.02)</f>
-        <v>11317.04</v>
+        <f>$H19 - ($H19 * 0.01)</f>
+        <v>10888.02</v>
       </c>
       <c r="H20" s="6">
-        <f>ROUND(MIN($G20, $B20), 0) - 2</f>
-        <v>11298</v>
+        <f t="shared" si="9"/>
+        <v>10848</v>
       </c>
       <c r="I20" s="6">
-        <f>ROUNDDOWN($F20/$H20, 5)</f>
-        <v>7.1599999999999997E-3</v>
+        <f t="shared" si="7"/>
+        <v>1.179E-2</v>
       </c>
       <c r="J20" s="6">
         <f>$H19 + ($H19* 0.005)</f>
-        <v>11605.74</v>
+        <v>11052.99</v>
       </c>
       <c r="K20">
-        <f>ROUND(MAX($J20,$C20), 0) + 2</f>
-        <v>11652</v>
+        <f t="shared" si="10"/>
+        <v>11055</v>
       </c>
       <c r="L20">
-        <f>$I19</f>
-        <v>7.79E-3</v>
+        <f t="shared" si="11"/>
+        <v>1.4540000000000001E-2</v>
       </c>
       <c r="N20" s="5">
-        <f>L20 * ($K20 - $H19)</f>
-        <v>0.81015999999999999</v>
+        <f t="shared" si="12"/>
+        <v>0.82878000000000007</v>
       </c>
       <c r="O20" s="7">
-        <f>$N20 / $F19</f>
-        <v>9.0017777777777769E-3</v>
+        <f t="shared" si="13"/>
+        <v>5.1798750000000005E-3</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="6"/>
       <c r="B21" s="6">
-        <v>11200</v>
+        <v>10676</v>
       </c>
       <c r="C21" s="6">
-        <v>11500</v>
+        <v>10677</v>
       </c>
       <c r="D21" s="6">
-        <f>$D20 - $F20</f>
-        <v>729</v>
+        <f t="shared" si="8"/>
+        <v>512</v>
       </c>
       <c r="E21" s="6" t="s">
         <v>24</v>
       </c>
       <c r="F21" s="6">
-        <f>$D21 * 0.1</f>
-        <v>72.900000000000006</v>
+        <f>$D21 * 0.2</f>
+        <v>102.4</v>
       </c>
       <c r="G21" s="6">
-        <f>$H20 - ($H20 * 0.005)</f>
-        <v>11241.51</v>
+        <f>$H20 - ($H20 * 0.015)</f>
+        <v>10685.28</v>
       </c>
       <c r="H21" s="6">
-        <f>ROUND(MIN($G21, $B21), 0) - 2</f>
-        <v>11198</v>
+        <f t="shared" si="9"/>
+        <v>10674</v>
       </c>
       <c r="I21" s="6">
-        <f>ROUNDDOWN($F21/$H21, 5)</f>
-        <v>6.5100000000000002E-3</v>
+        <f t="shared" si="7"/>
+        <v>9.5899999999999996E-3</v>
       </c>
       <c r="J21" s="6">
-        <f>$H20 + ($H20* 0.01)</f>
-        <v>11410.98</v>
+        <f>$H20 + ($H20* 0.005)</f>
+        <v>10902.24</v>
       </c>
       <c r="K21">
-        <f>ROUND(MAX($J21,$C21), 0) + 2</f>
-        <v>11502</v>
+        <f t="shared" si="10"/>
+        <v>10904</v>
       </c>
       <c r="L21">
-        <f>$I20</f>
-        <v>7.1599999999999997E-3</v>
+        <f t="shared" si="11"/>
+        <v>1.179E-2</v>
       </c>
       <c r="N21" s="5">
-        <f>L21 * ($K21 - $H20)</f>
-        <v>1.4606399999999999</v>
+        <f t="shared" si="12"/>
+        <v>0.66024000000000005</v>
       </c>
       <c r="O21" s="7">
-        <f>$N21 / $F20</f>
-        <v>1.8032592592592593E-2</v>
+        <f t="shared" si="13"/>
+        <v>5.1581250000000004E-3</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B22" s="6">
-        <v>11050</v>
+        <v>10600</v>
       </c>
       <c r="C22" s="6">
-        <v>11300</v>
+        <v>10601</v>
       </c>
       <c r="D22" s="6">
-        <f>$D21 - $F21</f>
-        <v>656.1</v>
+        <f t="shared" si="8"/>
+        <v>409.6</v>
       </c>
       <c r="E22" s="6" t="s">
         <v>24</v>
       </c>
       <c r="F22" s="6">
-        <f>$D22 * 0.1</f>
-        <v>65.61</v>
+        <f>$D22 * 0.15</f>
+        <v>61.44</v>
       </c>
       <c r="G22" s="6">
-        <f>$H21 - ($H21 * 0.01)</f>
-        <v>11086.02</v>
+        <f>$H21 - ($H21 * 0.005)</f>
+        <v>10620.63</v>
       </c>
       <c r="H22" s="6">
-        <f>ROUND(MIN($G22, $B22), 0) - 2</f>
-        <v>11048</v>
+        <f t="shared" si="9"/>
+        <v>10598</v>
       </c>
       <c r="I22" s="6">
-        <f>ROUNDDOWN($F22/$H22, 5)</f>
-        <v>5.9300000000000004E-3</v>
+        <f t="shared" si="7"/>
+        <v>5.79E-3</v>
       </c>
       <c r="J22" s="6">
-        <f>$H21 + ($H21* 0.005)</f>
-        <v>11253.99</v>
+        <f>$H21 + ($H21* 0.01)</f>
+        <v>10780.74</v>
       </c>
       <c r="K22">
-        <f>ROUND(MAX($J22,$C22), 0) + 2</f>
-        <v>11302</v>
+        <f t="shared" si="10"/>
+        <v>10783</v>
       </c>
       <c r="L22">
-        <f>$I21</f>
-        <v>6.5100000000000002E-3</v>
+        <f t="shared" si="11"/>
+        <v>9.5899999999999996E-3</v>
       </c>
       <c r="N22" s="5">
-        <f>L22 * ($K22 - $H21)</f>
-        <v>0.67703999999999998</v>
+        <f t="shared" si="12"/>
+        <v>1.04531</v>
       </c>
       <c r="O22" s="7">
-        <f>$N22 / $F21</f>
-        <v>9.2872427983539084E-3</v>
+        <f t="shared" si="13"/>
+        <v>1.0208105468749999E-2</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B23" s="6">
-        <v>10800</v>
+        <v>10525</v>
       </c>
       <c r="C23" s="6">
-        <v>11200</v>
+        <v>10526</v>
       </c>
       <c r="D23" s="6">
-        <f>$D22 - $F22</f>
-        <v>590.49</v>
+        <f t="shared" si="8"/>
+        <v>348.16</v>
       </c>
       <c r="E23" s="6" t="s">
         <v>24</v>
       </c>
       <c r="F23" s="6">
-        <f>$D23 * 0.1</f>
-        <v>59.049000000000007</v>
+        <f>$D23 * 0.15</f>
+        <v>52.224000000000004</v>
       </c>
       <c r="G23" s="6">
-        <f>$H22 - ($H22 * 0.02)</f>
-        <v>10827.04</v>
+        <f>$H22 - ($H22 * 0.005)</f>
+        <v>10545.01</v>
       </c>
       <c r="H23" s="6">
-        <f>ROUND(MIN($G23, $B23), 0) - 2</f>
-        <v>10798</v>
+        <f t="shared" si="9"/>
+        <v>10523</v>
       </c>
       <c r="I23" s="6">
-        <f>ROUNDDOWN($F23/$H23, 5)</f>
-        <v>5.4599999999999996E-3</v>
+        <f t="shared" si="7"/>
+        <v>4.96E-3</v>
       </c>
       <c r="J23" s="6">
         <f>$H22 + ($H22* 0.005)</f>
-        <v>11103.24</v>
+        <v>10650.99</v>
       </c>
       <c r="K23">
-        <f>ROUND(MAX($J23,$C23), 0) + 2</f>
-        <v>11202</v>
+        <f t="shared" si="10"/>
+        <v>10653</v>
       </c>
       <c r="L23">
-        <f>$I22</f>
-        <v>5.9300000000000004E-3</v>
+        <f t="shared" si="11"/>
+        <v>5.79E-3</v>
       </c>
       <c r="N23" s="5">
-        <f>L23 * ($K23 - $H22)</f>
-        <v>0.91322000000000003</v>
+        <f t="shared" si="12"/>
+        <v>0.31845000000000001</v>
       </c>
       <c r="O23" s="7">
-        <f>$N23 / $F22</f>
-        <v>1.3918914799573237E-2</v>
+        <f t="shared" si="13"/>
+        <v>5.1831054687500001E-3</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B24" s="6">
-        <v>10700</v>
+        <v>10400</v>
       </c>
       <c r="C24" s="6">
-        <v>11000</v>
+        <v>10401</v>
       </c>
       <c r="D24" s="6">
-        <f>$D23 - $F23</f>
-        <v>531.44100000000003</v>
+        <f t="shared" si="8"/>
+        <v>295.93600000000004</v>
       </c>
       <c r="E24" s="6" t="s">
         <v>24</v>
       </c>
       <c r="F24" s="6">
-        <f>$D24 * 0.1</f>
-        <v>53.144100000000009</v>
+        <f>$D24 * 0.15</f>
+        <v>44.390400000000007</v>
       </c>
       <c r="G24" s="6">
-        <f>$H23 - ($H23 * 0.005)</f>
-        <v>10744.01</v>
+        <f>$H23 - ($H23 * 0.01)</f>
+        <v>10417.77</v>
       </c>
       <c r="H24" s="6">
-        <f>ROUND(MIN($G24, $B24), 0) - 2</f>
-        <v>10698</v>
+        <f t="shared" si="9"/>
+        <v>10398</v>
       </c>
       <c r="I24" s="6">
-        <f>ROUNDDOWN($F24/$H24, 5)</f>
+        <f t="shared" si="7"/>
+        <v>4.2599999999999999E-3</v>
+      </c>
+      <c r="J24" s="6">
+        <f>$H23 + ($H23* 0.005)</f>
+        <v>10575.615</v>
+      </c>
+      <c r="K24">
+        <f t="shared" si="10"/>
+        <v>10578</v>
+      </c>
+      <c r="L24">
+        <f t="shared" si="11"/>
         <v>4.96E-3</v>
       </c>
-      <c r="J24" s="6">
-        <f>$H23 + ($H23* 0.01)</f>
-        <v>10905.98</v>
-      </c>
-      <c r="K24">
-        <f>ROUND(MAX($J24,$C24), 0) + 2</f>
-        <v>11002</v>
-      </c>
-      <c r="L24">
-        <f>$I23</f>
-        <v>5.4599999999999996E-3</v>
-      </c>
       <c r="N24" s="5">
-        <f>L24 * ($K24 - $H23)</f>
-        <v>1.1138399999999999</v>
+        <f t="shared" si="12"/>
+        <v>0.27279999999999999</v>
       </c>
       <c r="O24" s="7">
-        <f>$N24 / $F23</f>
-        <v>1.8862978204541987E-2</v>
+        <f t="shared" si="13"/>
+        <v>5.2236519607843134E-3</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
@@ -1529,8 +1530,8 @@
         <v>23</v>
       </c>
       <c r="F34" s="6">
-        <f>$D34 * 0.1</f>
-        <v>100</v>
+        <f>$D34 * 0.2</f>
+        <v>200</v>
       </c>
       <c r="G34" s="6">
         <f>$B34 - 2</f>
@@ -1542,7 +1543,7 @@
       </c>
       <c r="I34" s="6">
         <f>ROUNDDOWN($F34/$H34, 5)</f>
-        <v>7.7299999999999999E-3</v>
+        <v>1.546E-2</v>
       </c>
       <c r="J34" s="6" t="s">
         <v>7</v>
@@ -1562,7 +1563,7 @@
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B41" t="s">
         <v>17</v>
@@ -1643,8 +1644,8 @@
         <v>23</v>
       </c>
       <c r="F43" s="6">
-        <f>$D43 * 0.1</f>
-        <v>100</v>
+        <f>$D43 * 0.2</f>
+        <v>200</v>
       </c>
       <c r="G43" s="6">
         <f>$B43 - 2</f>
@@ -1656,7 +1657,7 @@
       </c>
       <c r="I43" s="6">
         <f>ROUNDDOWN($F43/$H43, 5)</f>
-        <v>8.5400000000000007E-3</v>
+        <v>1.7090000000000001E-2</v>
       </c>
       <c r="J43" s="6" t="s">
         <v>7</v>
@@ -1678,26 +1679,26 @@
       </c>
       <c r="D44" s="6">
         <f>$D43 - $F43</f>
-        <v>900</v>
+        <v>800</v>
       </c>
       <c r="E44" s="6" t="s">
         <v>24</v>
       </c>
       <c r="F44" s="6">
-        <f>$D44 * 0.1</f>
-        <v>90</v>
+        <f>$D44 * 0.2</f>
+        <v>160</v>
       </c>
       <c r="G44" s="6">
-        <f>$H43 - ($H43 * 0.01)</f>
-        <v>11583</v>
+        <f>$H43 - ($H43 * 0.005)</f>
+        <v>11641.5</v>
       </c>
       <c r="H44" s="6">
         <f>ROUND(MIN($G44, $B44), 0) - 2</f>
-        <v>11581</v>
+        <v>11640</v>
       </c>
       <c r="I44" s="6">
         <f>ROUNDDOWN($F44/$H44, 5)</f>
-        <v>7.77E-3</v>
+        <v>1.374E-2</v>
       </c>
       <c r="J44" s="6">
         <f>$H43 + ($H43* 0.005)</f>
@@ -1709,15 +1710,15 @@
       </c>
       <c r="L44">
         <f>$I43</f>
-        <v>8.5400000000000007E-3</v>
+        <v>1.7090000000000001E-2</v>
       </c>
       <c r="N44" s="5">
         <f>L44 * ($K44 - $H43)</f>
-        <v>0.52094000000000007</v>
+        <v>1.0424900000000001</v>
       </c>
       <c r="O44" s="7">
         <f>$N44 / $F43</f>
-        <v>5.2094000000000003E-3</v>
+        <v>5.2124500000000004E-3</v>
       </c>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.25">
@@ -1730,55 +1731,55 @@
       </c>
       <c r="D45" s="6">
         <f>$D44 - $F44</f>
-        <v>810</v>
+        <v>640</v>
       </c>
       <c r="E45" s="6" t="s">
         <v>24</v>
       </c>
       <c r="F45" s="6">
-        <f>$D45 * 0.1</f>
-        <v>81</v>
+        <f>$D45 * 0.2</f>
+        <v>128</v>
       </c>
       <c r="G45" s="6">
-        <f>$H44 - ($H44 * 0.02)</f>
-        <v>11349.38</v>
+        <f>$H44 - ($H44 * 0.01)</f>
+        <v>11523.6</v>
       </c>
       <c r="H45" s="6">
         <f>ROUND(MIN($G45, $B45), 0) - 2</f>
-        <v>11347</v>
+        <v>11522</v>
       </c>
       <c r="I45" s="6">
         <f>ROUNDDOWN($F45/$H45, 5)</f>
-        <v>7.1300000000000001E-3</v>
+        <v>1.11E-2</v>
       </c>
       <c r="J45" s="6">
         <f>$H44 + ($H44* 0.005)</f>
-        <v>11638.905000000001</v>
+        <v>11698.2</v>
       </c>
       <c r="K45">
         <f>ROUND(MAX($J45,$C45), 0) + 2</f>
-        <v>11641</v>
+        <v>11700</v>
       </c>
       <c r="L45">
         <f>$I44</f>
-        <v>7.77E-3</v>
+        <v>1.374E-2</v>
       </c>
       <c r="N45" s="5">
         <f>L45 * ($K45 - $H44)</f>
-        <v>0.4662</v>
+        <v>0.82440000000000002</v>
       </c>
       <c r="O45" s="7">
         <f>$N45 / $F44</f>
-        <v>5.1799999999999997E-3</v>
+        <v>5.1525E-3</v>
       </c>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A46" s="6"/>
       <c r="B46" s="6">
-        <v>11000</v>
+        <v>11701</v>
       </c>
       <c r="C46" s="6">
-        <v>11001</v>
+        <v>11702</v>
       </c>
       <c r="D46" s="6">
         <v>900</v>
@@ -1787,20 +1788,20 @@
         <v>23</v>
       </c>
       <c r="F46" s="6">
-        <f>$D46 * 0.1</f>
-        <v>90</v>
+        <f>$D46 * 0.2</f>
+        <v>180</v>
       </c>
       <c r="G46" s="6">
         <f>$K45 / 1.005</f>
-        <v>11583.084577114429</v>
+        <v>11641.791044776121</v>
       </c>
       <c r="H46" s="6">
         <f>ROUND(MIN($G46, $B46), 0) - 2</f>
-        <v>10998</v>
+        <v>11640</v>
       </c>
       <c r="I46" s="6">
         <f>ROUNDDOWN($F46/$H46, 5)</f>
-        <v>8.1799999999999998E-3</v>
+        <v>1.546E-2</v>
       </c>
       <c r="J46" s="6" t="s">
         <v>7</v>
@@ -1856,7 +1857,7 @@
     </row>
     <row r="54" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B54" t="s">
         <v>17</v>
@@ -1899,7 +1900,6 @@
       </c>
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A55" s="6"/>
       <c r="B55" s="6">
         <v>13000</v>
       </c>
@@ -1937,8 +1937,8 @@
         <v>23</v>
       </c>
       <c r="F56" s="6">
-        <f>$D56 * 0.1</f>
-        <v>100</v>
+        <f>$D56 * 0.2</f>
+        <v>200</v>
       </c>
       <c r="G56" s="6">
         <f>$B56 - 2</f>
@@ -1950,7 +1950,7 @@
       </c>
       <c r="I56" s="6">
         <f>ROUNDDOWN($F56/$H56, 5)</f>
-        <v>8.5400000000000007E-3</v>
+        <v>1.7090000000000001E-2</v>
       </c>
       <c r="J56" s="6" t="s">
         <v>7</v>
@@ -1965,33 +1965,33 @@
     <row r="57" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A57" s="6"/>
       <c r="B57" s="6">
-        <v>11702</v>
+        <v>11600</v>
       </c>
       <c r="C57" s="6">
-        <v>11703</v>
+        <v>11601</v>
       </c>
       <c r="D57" s="6">
         <f>$D56 - $F56</f>
-        <v>900</v>
+        <v>800</v>
       </c>
       <c r="E57" s="6" t="s">
         <v>24</v>
       </c>
       <c r="F57" s="6">
-        <f>$D57 * 0.1</f>
-        <v>90</v>
+        <f>$D57 * 0.2</f>
+        <v>160</v>
       </c>
       <c r="G57" s="6">
-        <f>$H56 - ($H56 * 0.01)</f>
-        <v>11583</v>
+        <f>$H56 - ($H56 * 0.005)</f>
+        <v>11641.5</v>
       </c>
       <c r="H57" s="6">
         <f>ROUND(MIN($G57, $B57), 0) - 2</f>
-        <v>11581</v>
+        <v>11598</v>
       </c>
       <c r="I57" s="6">
         <f>ROUNDDOWN($F57/$H57, 5)</f>
-        <v>7.77E-3</v>
+        <v>1.379E-2</v>
       </c>
       <c r="J57" s="6">
         <f>$H56 + ($H56* 0.005)</f>
@@ -2003,67 +2003,67 @@
       </c>
       <c r="L57">
         <f>$I56</f>
-        <v>8.5400000000000007E-3</v>
+        <v>1.7090000000000001E-2</v>
       </c>
       <c r="N57" s="5">
         <f>L57 * ($K57 - $H56)</f>
-        <v>0.52094000000000007</v>
+        <v>1.0424900000000001</v>
       </c>
       <c r="O57" s="7">
         <f>$N57 / $F56</f>
-        <v>5.2094000000000003E-3</v>
+        <v>5.2124500000000004E-3</v>
       </c>
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A58" s="6"/>
       <c r="B58" s="6">
-        <v>11582</v>
+        <v>11550</v>
       </c>
       <c r="C58" s="6">
-        <v>11583</v>
+        <v>11551</v>
       </c>
       <c r="D58" s="6">
         <f>$D57 - $F57</f>
-        <v>810</v>
+        <v>640</v>
       </c>
       <c r="E58" s="6" t="s">
         <v>24</v>
       </c>
       <c r="F58" s="6">
-        <f>$D58 * 0.1</f>
-        <v>81</v>
+        <f>$D58 * 0.2</f>
+        <v>128</v>
       </c>
       <c r="G58" s="6">
-        <f>$H57 - ($H57 * 0.02)</f>
-        <v>11349.38</v>
+        <f>$H57 - ($H57 * 0.01)</f>
+        <v>11482.02</v>
       </c>
       <c r="H58" s="6">
         <f>ROUND(MIN($G58, $B58), 0) - 2</f>
-        <v>11347</v>
+        <v>11480</v>
       </c>
       <c r="I58" s="6">
         <f>ROUNDDOWN($F58/$H58, 5)</f>
-        <v>7.1300000000000001E-3</v>
+        <v>1.1140000000000001E-2</v>
       </c>
       <c r="J58" s="6">
         <f>$H57 + ($H57* 0.005)</f>
-        <v>11638.905000000001</v>
+        <v>11655.99</v>
       </c>
       <c r="K58">
         <f>ROUND(MAX($J58,$C58), 0) + 2</f>
-        <v>11641</v>
+        <v>11658</v>
       </c>
       <c r="L58">
         <f>$I57</f>
-        <v>7.77E-3</v>
+        <v>1.379E-2</v>
       </c>
       <c r="N58" s="5">
         <f>L58 * ($K58 - $H57)</f>
-        <v>0.4662</v>
+        <v>0.82740000000000002</v>
       </c>
       <c r="O58" s="7">
         <f>$N58 / $F57</f>
-        <v>5.1799999999999997E-3</v>
+        <v>5.1712500000000005E-3</v>
       </c>
     </row>
     <row r="59" spans="1:15" x14ac:dyDescent="0.25">
@@ -2081,20 +2081,20 @@
         <v>23</v>
       </c>
       <c r="F59" s="6">
-        <f>$D59 * 0.1</f>
-        <v>90</v>
+        <f>$D59 * 0.2</f>
+        <v>180</v>
       </c>
       <c r="G59" s="6">
         <f>$K58 / 1.005</f>
-        <v>11583.084577114429</v>
+        <v>11600.000000000002</v>
       </c>
       <c r="H59" s="6">
         <f>ROUND(MIN($G59, $B59), 0) - 2</f>
-        <v>11581</v>
+        <v>11582</v>
       </c>
       <c r="I59" s="6">
         <f>ROUNDDOWN($F59/$H59, 5)</f>
-        <v>7.77E-3</v>
+        <v>1.554E-2</v>
       </c>
       <c r="J59" s="6" t="s">
         <v>7</v>
@@ -2118,9 +2118,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-  <ignoredErrors>
-    <ignoredError sqref="J6" formula="1"/>
-  </ignoredErrors>
 </worksheet>
 </file>
 
@@ -2128,8 +2125,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2191,272 +2188,272 @@
         <v>1000</v>
       </c>
       <c r="L2" s="5">
-        <f>$K2 * 0.1</f>
-        <v>100</v>
+        <f>$K2 * 0.2</f>
+        <v>200</v>
       </c>
       <c r="M2">
         <f>$L2/$F2</f>
-        <v>8.5899583387020577E-3</v>
+        <v>1.7179916677404115E-2</v>
       </c>
       <c r="N2" s="5">
         <f>$L2 *  $B2</f>
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="4">
-        <v>0.01</v>
+      <c r="A3" s="3">
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="B3" s="4">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="F3" s="5">
         <f t="shared" ref="F3:F22" si="0">$F2 - ($F2 * $A3)</f>
-        <v>11525.084999999999</v>
+        <v>11583.2925</v>
       </c>
       <c r="H3" s="4">
         <f t="shared" ref="H3:H22" si="1">($F$1 - $F3) / $F$1</f>
-        <v>1.4950000000000074E-2</v>
+        <v>9.9750000000000377E-3</v>
       </c>
       <c r="K3" s="5">
-        <f>$K2-($K2 * 0.1)</f>
-        <v>900</v>
+        <f>$K2-$L2</f>
+        <v>800</v>
       </c>
       <c r="L3" s="5">
-        <f t="shared" ref="L3:L22" si="2">$K3 * 0.1</f>
-        <v>90</v>
+        <f t="shared" ref="L3:L5" si="2">$K3 * 0.2</f>
+        <v>160</v>
       </c>
       <c r="M3">
         <f t="shared" ref="M3:M22" si="3">$L3/$F3</f>
-        <v>7.8090530351836891E-3</v>
+        <v>1.3812998333591248E-2</v>
       </c>
       <c r="N3" s="5">
         <f t="shared" ref="N3:N22" si="4">$L3 *  $B3</f>
-        <v>0.45</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
       <c r="B4" s="4">
-        <v>0.01</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="F4" s="5">
         <f t="shared" si="0"/>
-        <v>11294.583299999998</v>
+        <v>11467.459574999999</v>
       </c>
       <c r="H4" s="4">
         <f t="shared" si="1"/>
-        <v>3.4651000000000133E-2</v>
+        <v>1.9875250000000091E-2</v>
       </c>
       <c r="K4" s="5">
-        <f t="shared" ref="K4:K22" si="5">$K3-($K3 * 0.1)</f>
-        <v>810</v>
+        <f t="shared" ref="K4:K22" si="5">$K3-$L3</f>
+        <v>640</v>
       </c>
       <c r="L4" s="5">
         <f t="shared" si="2"/>
-        <v>81</v>
+        <v>128</v>
       </c>
       <c r="M4">
         <f t="shared" si="3"/>
-        <v>7.1715793180258374E-3</v>
+        <v>1.1162018855427272E-2</v>
       </c>
       <c r="N4" s="5">
         <f t="shared" si="4"/>
-        <v>0.81</v>
+        <v>0.64</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
-        <v>5.0000000000000001E-3</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="B5" s="4">
-        <v>5.0000000000000001E-3</v>
+        <v>0.01</v>
       </c>
       <c r="F5" s="5">
         <f t="shared" si="0"/>
-        <v>11238.110383499998</v>
+        <v>11295.447681374999</v>
       </c>
       <c r="H5" s="4">
         <f t="shared" si="1"/>
-        <v>3.9477745000000203E-2</v>
+        <v>3.4577121250000099E-2</v>
       </c>
       <c r="K5" s="5">
         <f t="shared" si="5"/>
-        <v>729</v>
+        <v>512</v>
       </c>
       <c r="L5" s="5">
         <f t="shared" si="2"/>
-        <v>72.900000000000006</v>
+        <v>102.4</v>
       </c>
       <c r="M5">
         <f t="shared" si="3"/>
-        <v>6.4868556645459848E-3</v>
+        <v>9.0655990703977854E-3</v>
       </c>
       <c r="N5" s="5">
         <f t="shared" si="4"/>
-        <v>0.36450000000000005</v>
+        <v>1.024</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="4">
-        <v>0.01</v>
+      <c r="A6" s="3">
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="B6" s="4">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="F6" s="5">
         <f t="shared" si="0"/>
-        <v>11125.729279664998</v>
+        <v>11238.970442968124</v>
       </c>
       <c r="H6" s="4">
         <f t="shared" si="1"/>
-        <v>4.9082967550000162E-2</v>
+        <v>3.940423564375007E-2</v>
       </c>
       <c r="K6" s="5">
         <f t="shared" si="5"/>
-        <v>656.1</v>
+        <v>409.6</v>
       </c>
       <c r="L6" s="5">
-        <f t="shared" si="2"/>
-        <v>65.61</v>
+        <f>$K6 * 0.15</f>
+        <v>61.44</v>
       </c>
       <c r="M6">
         <f t="shared" si="3"/>
-        <v>5.8971415132236214E-3</v>
+        <v>5.4666929067725334E-3</v>
       </c>
       <c r="N6" s="5">
         <f t="shared" si="4"/>
-        <v>0.32805000000000001</v>
+        <v>0.30719999999999997</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="4">
-        <v>0.02</v>
+      <c r="A7" s="3">
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="B7" s="4">
-        <v>0.01</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="F7" s="5">
         <f t="shared" si="0"/>
-        <v>10903.214694071698</v>
+        <v>11182.775590753283</v>
       </c>
       <c r="H7" s="4">
         <f t="shared" si="1"/>
-        <v>6.8101308199000218E-2</v>
+        <v>4.4207214465531386E-2</v>
       </c>
       <c r="K7" s="5">
         <f t="shared" si="5"/>
-        <v>590.49</v>
+        <v>348.16</v>
       </c>
       <c r="L7" s="5">
-        <f t="shared" si="2"/>
-        <v>59.049000000000007</v>
+        <f>$K7 * 0.15</f>
+        <v>52.224000000000004</v>
       </c>
       <c r="M7">
         <f t="shared" si="3"/>
-        <v>5.4157422060216939E-3</v>
+        <v>4.6700391665896023E-3</v>
       </c>
       <c r="N7" s="5">
         <f t="shared" si="4"/>
-        <v>0.59049000000000007</v>
+        <v>0.26112000000000002</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="3">
-        <v>5.0000000000000001E-3</v>
+      <c r="A8" s="4">
+        <v>0.01</v>
       </c>
       <c r="B8" s="4">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="F8" s="5">
         <f t="shared" si="0"/>
-        <v>10848.698620601339</v>
+        <v>11070.947834845751</v>
       </c>
       <c r="H8" s="4">
         <f t="shared" si="1"/>
-        <v>7.276080165800522E-2</v>
+        <v>5.3765142320876022E-2</v>
       </c>
       <c r="K8" s="5">
         <f t="shared" si="5"/>
-        <v>531.44100000000003</v>
+        <v>295.93600000000004</v>
       </c>
       <c r="L8" s="5">
-        <f t="shared" si="2"/>
-        <v>53.144100000000009</v>
+        <f>$K8 * 0.15</f>
+        <v>44.390400000000007</v>
       </c>
       <c r="M8">
         <f t="shared" si="3"/>
-        <v>4.8986612918789198E-3</v>
+        <v>4.009629587475921E-3</v>
       </c>
       <c r="N8" s="5">
         <f t="shared" si="4"/>
-        <v>0.26572050000000003</v>
+        <v>0.22195200000000004</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="4">
+      <c r="A9" s="3">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="B9" s="4">
         <v>0.01</v>
-      </c>
-      <c r="B9" s="4">
-        <v>5.0000000000000001E-3</v>
       </c>
       <c r="F9" s="5">
         <f t="shared" si="0"/>
-        <v>10740.211634395326</v>
+        <v>10904.883617323065</v>
       </c>
       <c r="H9" s="4">
         <f t="shared" si="1"/>
-        <v>8.2033193641425153E-2</v>
+        <v>6.7958665186062847E-2</v>
       </c>
       <c r="K9" s="5">
         <f t="shared" si="5"/>
-        <v>478.29690000000005</v>
+        <v>251.54560000000004</v>
       </c>
       <c r="L9" s="5">
-        <f t="shared" si="2"/>
-        <v>47.829690000000006</v>
+        <f>$K9 * 0.15</f>
+        <v>37.731840000000005</v>
       </c>
       <c r="M9">
         <f t="shared" si="3"/>
-        <v>4.4533284471626544E-3</v>
+        <v>3.460086446045211E-3</v>
       </c>
       <c r="N9" s="5">
         <f t="shared" si="4"/>
-        <v>0.23914845000000004</v>
+        <v>0.37731840000000005</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="4">
-        <v>0.02</v>
+      <c r="A10" s="3">
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="B10" s="4">
-        <v>0.01</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="F10" s="5">
         <f t="shared" si="0"/>
-        <v>10525.40740170742</v>
+        <v>10850.359199236449</v>
       </c>
       <c r="H10" s="4">
         <f t="shared" si="1"/>
-        <v>0.10039252976859658</v>
+        <v>7.2618871860132564E-2</v>
       </c>
       <c r="K10" s="5">
         <f t="shared" si="5"/>
-        <v>430.46721000000002</v>
+        <v>213.81376000000003</v>
       </c>
       <c r="L10" s="5">
-        <f t="shared" si="2"/>
-        <v>43.046721000000005</v>
+        <f>$K10 * 0.1</f>
+        <v>21.381376000000003</v>
       </c>
       <c r="M10">
         <f t="shared" si="3"/>
-        <v>4.0897914310677429E-3</v>
+        <v>1.9705684952351283E-3</v>
       </c>
       <c r="N10" s="5">
         <f t="shared" si="4"/>
-        <v>0.43046721000000004</v>
+        <v>0.10690688000000002</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
@@ -2468,27 +2465,27 @@
       </c>
       <c r="F11" s="5">
         <f t="shared" si="0"/>
-        <v>10472.780364698883</v>
+        <v>10796.107403240267</v>
       </c>
       <c r="H11" s="4">
         <f t="shared" si="1"/>
-        <v>0.10489056711975357</v>
+        <v>7.7255777500831915E-2</v>
       </c>
       <c r="K11" s="5">
         <f t="shared" si="5"/>
-        <v>387.42048900000003</v>
+        <v>192.43238400000001</v>
       </c>
       <c r="L11" s="5">
-        <f t="shared" si="2"/>
-        <v>38.742048900000007</v>
+        <f t="shared" ref="L11:L22" si="6">$K11 * 0.1</f>
+        <v>19.243238400000003</v>
       </c>
       <c r="M11">
         <f t="shared" si="3"/>
-        <v>3.699308832121577E-3</v>
+        <v>1.782423764534287E-3</v>
       </c>
       <c r="N11" s="5">
         <f t="shared" si="4"/>
-        <v>0.19371024450000005</v>
+        <v>9.621619200000002E-2</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
@@ -2500,59 +2497,59 @@
       </c>
       <c r="F12" s="5">
         <f t="shared" si="0"/>
-        <v>10368.052561051894</v>
+        <v>10688.146329207864</v>
       </c>
       <c r="H12" s="4">
         <f t="shared" si="1"/>
-        <v>0.11384166144855604</v>
+        <v>8.6483219725823568E-2</v>
       </c>
       <c r="K12" s="5">
         <f t="shared" si="5"/>
-        <v>348.67844010000005</v>
+        <v>173.18914560000002</v>
       </c>
       <c r="L12" s="5">
-        <f t="shared" si="2"/>
-        <v>34.867844010000006</v>
+        <f t="shared" si="6"/>
+        <v>17.318914560000003</v>
       </c>
       <c r="M12">
         <f t="shared" si="3"/>
-        <v>3.3630080292014336E-3</v>
+        <v>1.6203852404857156E-3</v>
       </c>
       <c r="N12" s="5">
         <f t="shared" si="4"/>
-        <v>0.17433922005000002</v>
+        <v>8.6594572800000019E-2</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" s="4">
-        <v>0.02</v>
+      <c r="A13" s="3">
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="B13" s="4">
         <v>0.01</v>
       </c>
       <c r="F13" s="5">
         <f t="shared" si="0"/>
-        <v>10160.691509830856</v>
+        <v>10527.824134269746</v>
       </c>
       <c r="H13" s="4">
         <f t="shared" si="1"/>
-        <v>0.13156482821958493</v>
+        <v>0.10018597142993627</v>
       </c>
       <c r="K13" s="5">
         <f t="shared" si="5"/>
-        <v>313.81059609000005</v>
+        <v>155.87023104000002</v>
       </c>
       <c r="L13" s="5">
-        <f t="shared" si="2"/>
-        <v>31.381059609000005</v>
+        <f t="shared" si="6"/>
+        <v>15.587023104000004</v>
       </c>
       <c r="M13">
         <f t="shared" si="3"/>
-        <v>3.0884767615115207E-3</v>
+        <v>1.4805550420681666E-3</v>
       </c>
       <c r="N13" s="5">
         <f t="shared" si="4"/>
-        <v>0.31381059609000006</v>
+        <v>0.15587023104000003</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
@@ -2564,283 +2561,283 @@
       </c>
       <c r="F14" s="5">
         <f t="shared" si="0"/>
-        <v>10109.888052281702</v>
+        <v>10475.185013598397</v>
       </c>
       <c r="H14" s="4">
         <f t="shared" si="1"/>
-        <v>0.13590700407848705</v>
+        <v>0.10468504157278659</v>
       </c>
       <c r="K14" s="5">
         <f t="shared" si="5"/>
-        <v>282.42953648100001</v>
+        <v>140.28320793600003</v>
       </c>
       <c r="L14" s="5">
-        <f t="shared" si="2"/>
-        <v>28.242953648100002</v>
+        <f t="shared" si="6"/>
+        <v>14.028320793600003</v>
       </c>
       <c r="M14">
         <f t="shared" si="3"/>
-        <v>2.7935970707139378E-3</v>
+        <v>1.3391955154385426E-3</v>
       </c>
       <c r="N14" s="5">
         <f t="shared" si="4"/>
-        <v>0.14121476824050003</v>
+        <v>7.014160396800001E-2</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="4">
-        <v>0.01</v>
+      <c r="A15" s="3">
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="B15" s="4">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="F15" s="5">
         <f t="shared" si="0"/>
-        <v>10008.789171758885</v>
+        <v>10422.809088530405</v>
       </c>
       <c r="H15" s="4">
         <f t="shared" si="1"/>
-        <v>0.14454793403770216</v>
+        <v>0.10916161636492269</v>
       </c>
       <c r="K15" s="5">
         <f t="shared" si="5"/>
-        <v>254.1865828329</v>
+        <v>126.25488714240002</v>
       </c>
       <c r="L15" s="5">
-        <f t="shared" si="2"/>
-        <v>25.41865828329</v>
+        <f t="shared" si="6"/>
+        <v>12.625488714240003</v>
       </c>
       <c r="M15">
         <f t="shared" si="3"/>
-        <v>2.5396337006490344E-3</v>
+        <v>1.2113326270298376E-3</v>
       </c>
       <c r="N15" s="5">
         <f t="shared" si="4"/>
-        <v>0.12709329141645001</v>
+        <v>6.3127443571200009E-2</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
       <c r="B16" s="4">
-        <v>0.01</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="F16" s="5">
         <f t="shared" si="0"/>
-        <v>9808.6133883237071</v>
+        <v>10318.5809976451</v>
       </c>
       <c r="H16" s="4">
         <f t="shared" si="1"/>
-        <v>0.16165697535694812</v>
+        <v>0.11807000020127349</v>
       </c>
       <c r="K16" s="5">
         <f t="shared" si="5"/>
-        <v>228.76792454961</v>
+        <v>113.62939842816002</v>
       </c>
       <c r="L16" s="5">
-        <f t="shared" si="2"/>
-        <v>22.876792454961002</v>
+        <f t="shared" si="6"/>
+        <v>11.362939842816003</v>
       </c>
       <c r="M16">
         <f t="shared" si="3"/>
-        <v>2.3323166638613583E-3</v>
+        <v>1.1012114791180343E-3</v>
       </c>
       <c r="N16" s="5">
         <f t="shared" si="4"/>
-        <v>0.22876792454961004</v>
+        <v>5.6814699214080014E-2</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
-        <v>5.0000000000000001E-3</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="B17" s="4">
-        <v>5.0000000000000001E-3</v>
+        <v>0.01</v>
       </c>
       <c r="F17" s="5">
         <f t="shared" si="0"/>
-        <v>9759.5703213820889</v>
+        <v>10163.802282680424</v>
       </c>
       <c r="H17" s="4">
         <f t="shared" si="1"/>
-        <v>0.16584869048016335</v>
+        <v>0.13129895019825433</v>
       </c>
       <c r="K17" s="5">
         <f t="shared" si="5"/>
-        <v>205.89113209464901</v>
+        <v>102.26645858534401</v>
       </c>
       <c r="L17" s="5">
-        <f t="shared" si="2"/>
-        <v>20.589113209464902</v>
+        <f t="shared" si="6"/>
+        <v>10.226645858534402</v>
       </c>
       <c r="M17">
         <f>$L17/$F17</f>
-        <v>2.1096331632916806E-3</v>
+        <v>1.0061830773667318E-3</v>
       </c>
       <c r="N17" s="5">
         <f>$L17 *  $B17</f>
-        <v>0.10294556604732451</v>
+        <v>0.10226645858534403</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A18" s="4">
-        <v>0.01</v>
+      <c r="A18" s="3">
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="B18" s="4">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="F18" s="5">
         <f t="shared" si="0"/>
-        <v>9661.9746181682676</v>
+        <v>10112.983271267023</v>
       </c>
       <c r="H18" s="4">
         <f t="shared" si="1"/>
-        <v>0.17419020357536175</v>
+        <v>0.13564245544726297</v>
       </c>
       <c r="K18" s="5">
         <f t="shared" si="5"/>
-        <v>185.30201888518411</v>
+        <v>92.039812726809615</v>
       </c>
       <c r="L18" s="5">
-        <f t="shared" si="2"/>
-        <v>18.530201888518413</v>
+        <f t="shared" si="6"/>
+        <v>9.2039812726809611</v>
       </c>
       <c r="M18">
         <f t="shared" si="3"/>
-        <v>1.9178483302651646E-3</v>
+        <v>9.1011534636186776E-4</v>
       </c>
       <c r="N18" s="5">
         <f t="shared" si="4"/>
-        <v>9.2651009442592067E-2</v>
+        <v>4.6019906363404806E-2</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A19" s="4">
-        <v>0.02</v>
+      <c r="A19" s="3">
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="B19" s="4">
-        <v>0.01</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="F19" s="5">
         <f t="shared" si="0"/>
-        <v>9468.7351258049021</v>
+        <v>10062.418354910687</v>
       </c>
       <c r="H19" s="4">
         <f t="shared" si="1"/>
-        <v>0.19070639950385451</v>
+        <v>0.1399642431700267</v>
       </c>
       <c r="K19" s="5">
         <f t="shared" si="5"/>
-        <v>166.77181699666571</v>
+        <v>82.835831454128652</v>
       </c>
       <c r="L19" s="5">
-        <f t="shared" si="2"/>
-        <v>16.677181699666573</v>
+        <f t="shared" si="6"/>
+        <v>8.2835831454128659</v>
       </c>
       <c r="M19">
         <f t="shared" si="3"/>
-        <v>1.7612892828965799E-3</v>
+        <v>8.232199112820916E-4</v>
       </c>
       <c r="N19" s="5">
         <f t="shared" si="4"/>
-        <v>0.16677181699666574</v>
+        <v>4.1417915727064332E-2</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A20" s="3">
-        <v>5.0000000000000001E-3</v>
+      <c r="A20" s="4">
+        <v>0.01</v>
       </c>
       <c r="B20" s="4">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="F20" s="5">
         <f t="shared" si="0"/>
-        <v>9421.3914501758773</v>
+        <v>9961.7941713615801</v>
       </c>
       <c r="H20" s="4">
         <f t="shared" si="1"/>
-        <v>0.19475286750633528</v>
+        <v>0.1485646007383265</v>
       </c>
       <c r="K20" s="5">
         <f t="shared" si="5"/>
-        <v>150.09463529699914</v>
+        <v>74.552248308715789</v>
       </c>
       <c r="L20" s="5">
-        <f t="shared" si="2"/>
-        <v>15.009463529699914</v>
+        <f t="shared" si="6"/>
+        <v>7.4552248308715789</v>
       </c>
       <c r="M20">
         <f t="shared" si="3"/>
-        <v>1.5931259845295696E-3</v>
+        <v>7.4838173752917413E-4</v>
       </c>
       <c r="N20" s="5">
         <f t="shared" si="4"/>
-        <v>7.5047317648499576E-2</v>
+        <v>3.7276124154357895E-2</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A21" s="4">
+      <c r="A21" s="3">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="B21" s="4">
         <v>0.01</v>
-      </c>
-      <c r="B21" s="4">
-        <v>5.0000000000000001E-3</v>
       </c>
       <c r="F21" s="5">
         <f t="shared" si="0"/>
-        <v>9327.1775356741182</v>
+        <v>9812.3672587911569</v>
       </c>
       <c r="H21" s="4">
         <f t="shared" si="1"/>
-        <v>0.20280533883127194</v>
+        <v>0.16133613172725156</v>
       </c>
       <c r="K21" s="5">
         <f t="shared" si="5"/>
-        <v>135.08517176729924</v>
+        <v>67.097023477844203</v>
       </c>
       <c r="L21" s="5">
-        <f t="shared" si="2"/>
-        <v>13.508517176729924</v>
+        <f t="shared" si="6"/>
+        <v>6.7097023477844209</v>
       </c>
       <c r="M21">
         <f>$L21/$F21</f>
-        <v>1.4482963495723363E-3</v>
+        <v>6.8380057236168195E-4</v>
       </c>
       <c r="N21" s="5">
         <f t="shared" si="4"/>
-        <v>6.7542585883649628E-2</v>
+        <v>6.7097023477844214E-2</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
-        <v>0.02</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="B22" s="4">
-        <v>0.01</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="F22" s="5">
         <f t="shared" si="0"/>
-        <v>9140.6339849606356</v>
+        <v>9763.305422497202</v>
       </c>
       <c r="H22" s="4">
         <f t="shared" si="1"/>
-        <v>0.21874923205464653</v>
+        <v>0.16552945106861522</v>
       </c>
       <c r="K22" s="5">
         <f t="shared" si="5"/>
-        <v>121.57665459056932</v>
+        <v>60.387321130059782</v>
       </c>
       <c r="L22" s="5">
-        <f t="shared" si="2"/>
-        <v>12.157665459056933</v>
+        <f t="shared" si="6"/>
+        <v>6.0387321130059783</v>
       </c>
       <c r="M22">
         <f t="shared" si="3"/>
-        <v>1.3300680761378599E-3</v>
+        <v>6.1851308052815435E-4</v>
       </c>
       <c r="N22" s="5">
         <f t="shared" si="4"/>
-        <v>0.12157665459056934</v>
+        <v>3.0193660565029892E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>